<commit_message>
update 202212 report data.
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/202212/jsliu__bank_test_&_city_(HF)(202212)_DASHBOARD.xlsx
+++ b/lib/report/benchmark_report/web14/exl/202212/jsliu__bank_test_&_city_(HF)(202212)_DASHBOARD.xlsx
@@ -43,7 +43,7 @@
     <t>As of date: Dec, 2022</t>
   </si>
   <si>
-    <t>Printed on: 2023-02-09 14:08</t>
+    <t>Printed on: 2023-02-10 14:32</t>
   </si>
   <si>
     <t>Previous Cycle: Sep, 2022</t>
@@ -322,7 +322,7 @@
   </si>
   <si>
     <t xml:space="preserve">Earnings-at-Risk (EaR)
- NII: 5,602
+ NII: 5,604
  12 months horizon</t>
   </si>
   <si>
@@ -389,7 +389,7 @@
   </si>
   <si>
     <t xml:space="preserve">Earnings-at-Risk (EaR)
- NII: 10,681
+ NII: 10,684
  24 months horizon</t>
   </si>
   <si>
@@ -415,7 +415,7 @@
   </si>
   <si>
     <t xml:space="preserve">EVE at Risk
- EVE: 24,687
+ EVE: 24,690
  Duration: 4.67</t>
   </si>
   <si>
@@ -2592,13 +2592,13 @@
         <v>26</v>
       </c>
       <c r="B20" s="63">
-        <v>140621</v>
+        <v>140621.017</v>
       </c>
       <c r="C20" s="65">
-        <v>4.93546648035313</v>
+        <v>4.9354966622094594</v>
       </c>
       <c r="D20" s="66">
-        <v>2.30615760719703</v>
+        <v>2.30556272893264</v>
       </c>
       <c r="E20" s="62">
         <v>141538</v>
@@ -2614,13 +2614,13 @@
       </c>
       <c r="J20" s="45"/>
       <c r="K20" s="58">
-        <v>17.5412243670937</v>
+        <v>17.543308486614002</v>
       </c>
       <c r="L20" s="15">
         <v>17.704968378931298</v>
       </c>
       <c r="M20" s="15">
-        <v>-0.16374401183759701</v>
+        <v>-0.16165989231729583</v>
       </c>
     </row>
     <row r="21">
@@ -2650,13 +2650,13 @@
       </c>
       <c r="J21" s="45"/>
       <c r="K21" s="58">
-        <v>4.67110368576127</v>
+        <v>4.66836062820837</v>
       </c>
       <c r="L21" s="15">
         <v>4.85617165336736</v>
       </c>
       <c r="M21" s="15">
-        <v>-0.18506796760608957</v>
+        <v>-0.1878110251589904</v>
       </c>
     </row>
     <row r="22">
@@ -2667,10 +2667,10 @@
         <v>16619</v>
       </c>
       <c r="C22" s="72">
-        <v>1.9267140678204502</v>
+        <v>1.92724810999458</v>
       </c>
       <c r="D22" s="70">
-        <v>1.46271404410312</v>
+        <v>1.46269349635631</v>
       </c>
       <c r="E22" s="67">
         <v>23708</v>
@@ -2686,13 +2686,13 @@
       </c>
       <c r="J22" s="45"/>
       <c r="K22" s="59">
-        <v>-22.8685861410605</v>
+        <v>-22.8751582644323</v>
       </c>
       <c r="L22" s="15">
         <v>-23.6586049659914</v>
       </c>
       <c r="M22" s="15">
-        <v>0.79001882493090037</v>
+        <v>0.78344670155910023</v>
       </c>
     </row>
     <row r="23">
@@ -2700,13 +2700,13 @@
         <v>32</v>
       </c>
       <c r="B23" s="68">
-        <v>106497</v>
+        <v>106497.017</v>
       </c>
       <c r="C23" s="70">
-        <v>5.65170446905198</v>
-      </c>
-      <c r="D23" s="72">
-        <v>2.81703786070771</v>
+        <v>5.6516608695246395</v>
+      </c>
+      <c r="D23" s="70">
+        <v>2.81624329385909</v>
       </c>
       <c r="E23" s="67">
         <v>104979</v>
@@ -2722,13 +2722,13 @@
       </c>
       <c r="J23" s="45"/>
       <c r="K23" s="58">
-        <v>7.2130362071470193</v>
+        <v>7.20918749362305</v>
       </c>
       <c r="L23" s="15">
         <v>8.48120704617382</v>
       </c>
       <c r="M23" s="15">
-        <v>-1.2681708390268005</v>
+        <v>-1.2720195525507698</v>
       </c>
     </row>
     <row r="24">
@@ -2736,13 +2736,13 @@
         <v>34</v>
       </c>
       <c r="B24" s="68">
-        <v>89439</v>
+        <v>89439.018</v>
       </c>
       <c r="C24" s="72">
-        <v>5.4551146591313406</v>
+        <v>5.45513984567675</v>
       </c>
       <c r="D24" s="70">
-        <v>2.94234700490486</v>
+        <v>2.9414018645567</v>
       </c>
       <c r="E24" s="67">
         <v>88990</v>
@@ -2758,13 +2758,13 @@
       </c>
       <c r="J24" s="45"/>
       <c r="K24" s="60">
-        <v>915.765411670193</v>
+        <v>915.825026118946</v>
       </c>
       <c r="L24" s="28">
         <v>900.441476372895</v>
       </c>
       <c r="M24" s="28">
-        <v>15.323935297298021</v>
+        <v>15.383549746051017</v>
       </c>
     </row>
     <row r="25">
@@ -2772,13 +2772,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="68">
-        <v>17058</v>
+        <v>17057.999</v>
       </c>
       <c r="C25" s="70">
-        <v>6.67812880335631</v>
+        <v>6.6777270565712907</v>
       </c>
       <c r="D25" s="72">
-        <v>2.17478046521023</v>
+        <v>2.17473224911237</v>
       </c>
       <c r="E25" s="67">
         <v>15989</v>
@@ -2794,13 +2794,13 @@
       </c>
       <c r="J25" s="45"/>
       <c r="K25" s="58">
-        <v>4.0949647963934</v>
+        <v>4.09612969763073</v>
       </c>
       <c r="L25" s="15">
         <v>4.20927007445733</v>
       </c>
       <c r="M25" s="15">
-        <v>-0.11430527806392998</v>
+        <v>-0.11314037682659972</v>
       </c>
     </row>
     <row r="26" ht="15">
@@ -2808,13 +2808,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="63">
-        <v>124823</v>
+        <v>124823.003</v>
       </c>
       <c r="C26" s="65">
-        <v>0.538257319138784</v>
+        <v>0.537152610084218</v>
       </c>
       <c r="D26" s="66">
-        <v>1.80306925229776</v>
+        <v>1.80285892554534</v>
       </c>
       <c r="E26" s="62">
         <v>126134</v>
@@ -2830,13 +2830,13 @@
       </c>
       <c r="J26" s="45"/>
       <c r="K26" s="61">
-        <v>5602.16442647506</v>
+        <v>5603.78112555724</v>
       </c>
       <c r="L26" s="28">
         <v>5815.23232341052</v>
       </c>
       <c r="M26" s="28">
-        <v>-213.06789693545943</v>
+        <v>-211.45119785328006</v>
       </c>
     </row>
     <row r="27">
@@ -2844,13 +2844,13 @@
         <v>40</v>
       </c>
       <c r="B27" s="71">
-        <v>120243</v>
+        <v>120242.999</v>
       </c>
       <c r="C27" s="72">
-        <v>0.546637665111986</v>
+        <v>0.545636784225584</v>
       </c>
       <c r="D27" s="70">
-        <v>1.85079208093601</v>
+        <v>1.85057233385735</v>
       </c>
       <c r="E27" s="67">
         <v>125524</v>
@@ -2866,13 +2866,13 @@
       </c>
       <c r="J27" s="45"/>
       <c r="K27" s="61">
-        <v>1135.84533810065</v>
+        <v>1137.05809946493</v>
       </c>
       <c r="L27" s="28">
         <v>1518.9642274414</v>
       </c>
       <c r="M27" s="28">
-        <v>-383.11888934075</v>
+        <v>-381.90612797647009</v>
       </c>
     </row>
     <row r="28">
@@ -2883,10 +2883,10 @@
         <v>83018</v>
       </c>
       <c r="C28" s="72">
-        <v>0.362187791786938</v>
+        <v>0.36069566984219803</v>
       </c>
       <c r="D28" s="72">
-        <v>2.38207397259864</v>
+        <v>2.38175694478556</v>
       </c>
       <c r="E28" s="67">
         <v>88201</v>
@@ -2902,13 +2902,13 @@
       </c>
       <c r="J28" s="45"/>
       <c r="K28" s="58">
-        <v>4.60104108551501</v>
+        <v>4.60532493145209</v>
       </c>
       <c r="L28" s="15">
         <v>6.02576525365789</v>
       </c>
       <c r="M28" s="15">
-        <v>-1.4247241681428804</v>
+        <v>-1.4204403222058</v>
       </c>
     </row>
     <row r="29">
@@ -2916,13 +2916,13 @@
         <v>44</v>
       </c>
       <c r="B29" s="71">
-        <v>37225</v>
+        <v>37224.999</v>
       </c>
       <c r="C29" s="72">
-        <v>0.951762330869526</v>
+        <v>0.951879764993416</v>
       </c>
       <c r="D29" s="70">
-        <v>0.737428575316329</v>
+        <v>0.737415558666343</v>
       </c>
       <c r="E29" s="67">
         <v>37323</v>
@@ -2939,13 +2939,13 @@
         <v>45</v>
       </c>
       <c r="B30" s="68">
-        <v>4199</v>
+        <v>4199.004</v>
       </c>
       <c r="C30" s="72">
-        <v>0.347116118313884</v>
+        <v>0.342938125326863</v>
       </c>
       <c r="D30" s="72">
-        <v>0.66356921704137</v>
+        <v>0.663581364719357</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>46</v>
@@ -3028,7 +3028,7 @@
         <v>400</v>
       </c>
       <c r="D35" s="19">
-        <v>0.0721303620714702</v>
+        <v>0.0720918749362305</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>57</v>
@@ -3052,7 +3052,7 @@
         <v>300</v>
       </c>
       <c r="D36" s="19">
-        <v>0.0560613395931156</v>
+        <v>0.0560271290432385</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>57</v>
@@ -3076,7 +3076,7 @@
         <v>200</v>
       </c>
       <c r="D37" s="19">
-        <v>0.039678797388226</v>
+        <v>0.0396517140342517</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>57</v>
@@ -3108,7 +3108,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="19">
-        <v>0.020817395128413</v>
+        <v>0.0208057514968031</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>57</v>
@@ -3166,7 +3166,7 @@
         <v>-100</v>
       </c>
       <c r="D40" s="19">
-        <v>-0.0221122048653095</v>
+        <v>-0.0221050584631583</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>57</v>
@@ -3198,7 +3198,7 @@
         <v>-200</v>
       </c>
       <c r="D41" s="19">
-        <v>-0.0459949505910554</v>
+        <v>-0.0459758490133388</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>57</v>
@@ -3252,7 +3252,7 @@
         <v>67</v>
       </c>
       <c r="D43" s="19">
-        <v>0.034631821104308</v>
+        <v>0.0346064322747612</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>57</v>
@@ -3314,7 +3314,7 @@
         <v>400</v>
       </c>
       <c r="D45" s="19">
-        <v>0.112453631813822</v>
+        <v>0.112392266037563</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>57</v>
@@ -3346,7 +3346,7 @@
         <v>300</v>
       </c>
       <c r="D46" s="19">
-        <v>0.0883316509268715</v>
+        <v>0.0882774689802363</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>57</v>
@@ -3378,7 +3378,7 @@
         <v>200</v>
       </c>
       <c r="D47" s="19">
-        <v>0.0628510983601754</v>
+        <v>0.0628096688695394</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>57</v>
@@ -3410,7 +3410,7 @@
         <v>100</v>
       </c>
       <c r="D48" s="19">
-        <v>0.0327497493573731</v>
+        <v>0.0327354849332773</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>57</v>
@@ -3466,7 +3466,7 @@
         <v>-100</v>
       </c>
       <c r="D50" s="19">
-        <v>-0.0351894510558918</v>
+        <v>-0.0351775880960924</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>57</v>
@@ -3498,7 +3498,7 @@
         <v>-200</v>
       </c>
       <c r="D51" s="19">
-        <v>-0.0743953789622909</v>
+        <v>-0.074364645368532</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>57</v>
@@ -3544,7 +3544,7 @@
         <v>67</v>
       </c>
       <c r="D53" s="19">
-        <v>0.0413740549447014</v>
+        <v>0.0413423340460545</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>57</v>
@@ -3595,7 +3595,7 @@
         <v>400</v>
       </c>
       <c r="D55" s="19">
-        <v>-0.228685861410605</v>
+        <v>-0.228751582644323</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>57</v>
@@ -3619,7 +3619,7 @@
         <v>300</v>
       </c>
       <c r="D56" s="19">
-        <v>-0.166379821983069</v>
+        <v>-0.166440467163279</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>57</v>
@@ -3643,7 +3643,7 @@
         <v>200</v>
       </c>
       <c r="D57" s="19">
-        <v>-0.104730579047761</v>
+        <v>-0.104776741352632</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>57</v>
@@ -3675,7 +3675,7 @@
         <v>100</v>
       </c>
       <c r="D58" s="19">
-        <v>-0.0499840855492294</v>
+        <v>-0.0500038327141156</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>57</v>
@@ -3691,13 +3691,13 @@
       </c>
       <c r="J58" s="45"/>
       <c r="K58" s="15">
-        <v>7.8041421168346909</v>
+        <v>7.8042447741574</v>
       </c>
       <c r="L58" s="15">
-        <v>7.8288089648115591</v>
+        <v>7.82891202706346</v>
       </c>
       <c r="M58" s="15">
-        <v>25.2028458491224</v>
+        <v>25.2128308079875</v>
       </c>
     </row>
     <row r="59" ht="15">
@@ -3717,13 +3717,13 @@
       </c>
       <c r="J59" s="45"/>
       <c r="K59" s="15">
-        <v>18.092224534714298</v>
+        <v>18.092554084594</v>
       </c>
       <c r="L59" s="15">
-        <v>18.16656048182</v>
+        <v>18.166891985577</v>
       </c>
       <c r="M59" s="15">
-        <v>40.813697746016096</v>
+        <v>40.8238246105632</v>
       </c>
     </row>
     <row r="60" ht="15">
@@ -3733,7 +3733,7 @@
         <v>-100</v>
       </c>
       <c r="D60" s="19">
-        <v>0.0430980873185049</v>
+        <v>0.0431157477391154</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>57</v>
@@ -3749,13 +3749,13 @@
       </c>
       <c r="J60" s="45"/>
       <c r="K60" s="15">
-        <v>2.31111719823051</v>
+        <v>2.31116498749648</v>
       </c>
       <c r="L60" s="15">
-        <v>2.31725395626537</v>
+        <v>2.31730188347427</v>
       </c>
       <c r="M60" s="15">
-        <v>26.5638157029415</v>
+        <v>26.5780875530575</v>
       </c>
     </row>
     <row r="61" ht="15">
@@ -3765,7 +3765,7 @@
         <v>-200</v>
       </c>
       <c r="D61" s="19">
-        <v>0.069107962235365</v>
+        <v>0.0691119416445477</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>57</v>
@@ -3793,7 +3793,7 @@
         <v>67</v>
       </c>
       <c r="D63" s="19">
-        <v>-0.0831664613020303</v>
+        <v>-0.0831690682530268</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>57</v>
@@ -3842,20 +3842,20 @@
         <v>13100</v>
       </c>
       <c r="F66" s="16">
-        <v>13236.851525381</v>
+        <v>13236.9400546305</v>
       </c>
       <c r="G66" s="42">
-        <v>13349.1075948985</v>
+        <v>13349.2870445035</v>
       </c>
       <c r="H66" s="42"/>
       <c r="I66" s="16">
-        <v>13461.4644358334</v>
+        <v>13461.7427823901</v>
       </c>
       <c r="J66" s="16">
-        <v>13570.3639992764</v>
+        <v>13570.7480648864</v>
       </c>
       <c r="K66" s="16">
-        <v>13672.81511447</v>
+        <v>13673.3041714</v>
       </c>
     </row>
     <row r="67">
@@ -3865,23 +3865,23 @@
       <c r="C67" s="44"/>
       <c r="D67" s="44"/>
       <c r="E67" s="16">
-        <v>207.349356204663</v>
+        <v>207.349645340184</v>
       </c>
       <c r="F67" s="16">
-        <v>1613.40566644065</v>
+        <v>1613.40565657602</v>
       </c>
       <c r="G67" s="42">
-        <v>208.060144157945</v>
+        <v>208.060433806942</v>
       </c>
       <c r="H67" s="42"/>
       <c r="I67" s="16">
-        <v>247.12825661806</v>
+        <v>247.128459750317</v>
       </c>
       <c r="J67" s="16">
-        <v>272.55215200818</v>
+        <v>272.551887845893</v>
       </c>
       <c r="K67" s="16">
-        <v>2434.72792815442</v>
+        <v>2434.7284369987</v>
       </c>
     </row>
     <row r="68">
@@ -3891,23 +3891,23 @@
       <c r="C68" s="44"/>
       <c r="D68" s="44"/>
       <c r="E68" s="16">
-        <v>1937.19853524096</v>
+        <v>1936.58608054635</v>
       </c>
       <c r="F68" s="16">
-        <v>1660.05501576672</v>
+        <v>1658.91798905265</v>
       </c>
       <c r="G68" s="42">
-        <v>1865.75178856004</v>
+        <v>1864.19802511673</v>
       </c>
       <c r="H68" s="42"/>
       <c r="I68" s="16">
-        <v>1931.9491893882</v>
+        <v>1931.31043378126</v>
       </c>
       <c r="J68" s="16">
-        <v>1999.39644746939</v>
+        <v>1999.15349596587</v>
       </c>
       <c r="K68" s="16">
-        <v>1893.33288243763</v>
+        <v>1893.18904989299</v>
       </c>
     </row>
     <row r="69">
@@ -3916,24 +3916,24 @@
       </c>
       <c r="C69" s="44"/>
       <c r="D69" s="44"/>
-      <c r="E69" s="16">
-        <v>333.333333333333</v>
-      </c>
-      <c r="F69" s="16">
-        <v>666.666666666663</v>
-      </c>
-      <c r="G69" s="42">
-        <v>666.666666666663</v>
+      <c r="E69" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G69" s="42" t="s">
+        <v>46</v>
       </c>
       <c r="H69" s="42"/>
-      <c r="I69" s="16">
-        <v>666.666666666673</v>
-      </c>
-      <c r="J69" s="16">
-        <v>666.666666666663</v>
-      </c>
-      <c r="K69" s="16">
-        <v>666.666666666663</v>
+      <c r="I69" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K69" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="70">
@@ -3943,23 +3943,23 @@
       <c r="C70" s="44"/>
       <c r="D70" s="44"/>
       <c r="E70" s="16">
-        <v>4622.98866130839</v>
+        <v>4623.81378528582</v>
       </c>
       <c r="F70" s="16">
-        <v>4600.05359122427</v>
+        <v>4600.87718088603</v>
       </c>
       <c r="G70" s="42">
-        <v>4580.4976115504</v>
+        <v>4581.3145533773</v>
       </c>
       <c r="H70" s="42"/>
       <c r="I70" s="16">
-        <v>6583.71868809411</v>
+        <v>6584.51757328417</v>
       </c>
       <c r="J70" s="16">
-        <v>6555.95915484407</v>
+        <v>6556.77137905015</v>
       </c>
       <c r="K70" s="16">
-        <v>6530.81449052776</v>
+        <v>6531.64105017944</v>
       </c>
     </row>
     <row r="71">
@@ -3969,23 +3969,23 @@
       <c r="C71" s="44"/>
       <c r="D71" s="44"/>
       <c r="E71" s="16">
-        <v>136.851525380826</v>
+        <v>136.940054630411</v>
       </c>
       <c r="F71" s="16">
-        <v>112.256069815983</v>
+        <v>112.346990171524</v>
       </c>
       <c r="G71" s="42">
-        <v>112.356839883678</v>
+        <v>112.455736835422</v>
       </c>
       <c r="H71" s="42"/>
       <c r="I71" s="16">
-        <v>108.899562086538</v>
+        <v>109.005281139708</v>
       </c>
       <c r="J71" s="16">
-        <v>102.451115796415</v>
+        <v>102.556107116348</v>
       </c>
       <c r="K71" s="16">
-        <v>95.2742607676718</v>
+        <v>95.3787549543705</v>
       </c>
     </row>
     <row r="72">
@@ -4021,23 +4021,23 @@
       <c r="C73" s="45"/>
       <c r="D73" s="45"/>
       <c r="E73" s="16">
-        <v>20337.7214114682</v>
+        <v>15380.8757805169</v>
       </c>
       <c r="F73" s="16">
-        <v>21889.2885352952</v>
+        <v>16621.6106904307</v>
       </c>
       <c r="G73" s="42">
-        <v>20782.4406457172</v>
+        <v>15534.0012402625</v>
       </c>
       <c r="H73" s="42"/>
       <c r="I73" s="16">
-        <v>22999.8267986869</v>
+        <v>15749.1869570614</v>
       </c>
       <c r="J73" s="16">
-        <v>23167.3895360611</v>
+        <v>15945.0095558145</v>
       </c>
       <c r="K73" s="16">
-        <v>25293.6313430241</v>
+        <v>18096.600413246</v>
       </c>
     </row>
     <row r="74">
@@ -4047,23 +4047,23 @@
       <c r="C74" s="44"/>
       <c r="D74" s="44"/>
       <c r="E74" s="16">
-        <v>207.349356204654</v>
+        <v>207.349645340184</v>
       </c>
       <c r="F74" s="16">
-        <v>1613.40566644054</v>
+        <v>1613.40565657591</v>
       </c>
       <c r="G74" s="42">
-        <v>208.060144157792</v>
+        <v>208.060433806788</v>
       </c>
       <c r="H74" s="42"/>
       <c r="I74" s="16">
-        <v>247.128256618752</v>
+        <v>247.128459751007</v>
       </c>
       <c r="J74" s="16">
-        <v>272.552152007986</v>
+        <v>272.551887845698</v>
       </c>
       <c r="K74" s="16">
-        <v>2434.72792815398</v>
+        <v>2434.72843699826</v>
       </c>
     </row>
     <row r="75">
@@ -4073,23 +4073,23 @@
       <c r="C75" s="44"/>
       <c r="D75" s="44"/>
       <c r="E75" s="16">
-        <v>1955.01263724983</v>
+        <v>1954.40019552537</v>
       </c>
       <c r="F75" s="16">
-        <v>1678.53557759155</v>
+        <v>1677.39856526427</v>
       </c>
       <c r="G75" s="42">
-        <v>1884.96699133093</v>
+        <v>1883.4132516961</v>
       </c>
       <c r="H75" s="42"/>
       <c r="I75" s="16">
-        <v>1952.92066048745</v>
+        <v>1952.28186965485</v>
       </c>
       <c r="J75" s="16">
-        <v>2021.2065837925</v>
+        <v>2020.96355722983</v>
       </c>
       <c r="K75" s="16">
-        <v>1917.39732064392</v>
+        <v>1917.25330725089</v>
       </c>
     </row>
     <row r="76">
@@ -4099,23 +4099,23 @@
       <c r="C76" s="44"/>
       <c r="D76" s="44"/>
       <c r="E76" s="16">
-        <v>333.333333333333</v>
+        <v>333.333</v>
       </c>
       <c r="F76" s="16">
-        <v>666.666666666666</v>
+        <v>666.666</v>
       </c>
       <c r="G76" s="42">
-        <v>666.666666666666</v>
+        <v>666.666</v>
       </c>
       <c r="H76" s="42"/>
       <c r="I76" s="16">
-        <v>666.666666666666</v>
+        <v>666.666</v>
       </c>
       <c r="J76" s="16">
-        <v>666.666666666666</v>
+        <v>666.666</v>
       </c>
       <c r="K76" s="16">
-        <v>666.666666666666</v>
+        <v>666.666</v>
       </c>
     </row>
     <row r="77">
@@ -4125,23 +4125,23 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="16">
-        <v>4622.98866130831</v>
+        <v>4623.81378528572</v>
       </c>
       <c r="F77" s="16">
-        <v>4600.05359155425</v>
+        <v>4600.87718121602</v>
       </c>
       <c r="G77" s="42">
-        <v>4580.49761042952</v>
+        <v>4581.31455225658</v>
       </c>
       <c r="H77" s="42"/>
       <c r="I77" s="16">
-        <v>6583.71868677884</v>
+        <v>6584.51757196881</v>
       </c>
       <c r="J77" s="16">
-        <v>6555.95915550386</v>
+        <v>6556.77137970991</v>
       </c>
       <c r="K77" s="16">
-        <v>6530.81449019453</v>
+        <v>6531.64104984629</v>
       </c>
     </row>
     <row r="78">
@@ -4151,23 +4151,23 @@
       <c r="C78" s="44"/>
       <c r="D78" s="44"/>
       <c r="E78" s="16">
-        <v>-17.8141020089245</v>
+        <v>-17.8141149790485</v>
       </c>
       <c r="F78" s="16">
-        <v>-18.4805618562523</v>
+        <v>-18.480576242902</v>
       </c>
       <c r="G78" s="42">
-        <v>-19.2152027010538</v>
+        <v>-19.215226509743</v>
       </c>
       <c r="H78" s="42"/>
       <c r="I78" s="16">
-        <v>-20.9714711411306</v>
+        <v>-20.9714359154992</v>
       </c>
       <c r="J78" s="16">
-        <v>-21.8101363799145</v>
+        <v>-21.8100613207209</v>
       </c>
       <c r="K78" s="16">
-        <v>-24.0644382121033</v>
+        <v>-24.064257363565</v>
       </c>
     </row>
     <row r="79">
@@ -4203,23 +4203,23 @@
       <c r="C80" s="46"/>
       <c r="D80" s="46"/>
       <c r="E80" s="16">
-        <v>7100.86988608712</v>
+        <v>17542.6256213826</v>
       </c>
       <c r="F80" s="16">
-        <v>8540.18094039677</v>
+        <v>19912.4149119408</v>
       </c>
       <c r="G80" s="42">
-        <v>7320.97620988384</v>
+        <v>17625.4749268862</v>
       </c>
       <c r="H80" s="42"/>
       <c r="I80" s="16">
-        <v>9429.46279941057</v>
+        <v>17948.5972877827</v>
       </c>
       <c r="J80" s="16">
-        <v>9494.57442159112</v>
+        <v>18238.5250002303</v>
       </c>
       <c r="K80" s="16">
-        <v>11525.541967447</v>
+        <v>22448.5821578282</v>
       </c>
     </row>
     <row r="81">
@@ -4229,23 +4229,23 @@
       <c r="C81" s="46"/>
       <c r="D81" s="46"/>
       <c r="E81" s="30">
-        <v>2.86411689521537</v>
+        <v>0.87677159123599</v>
       </c>
       <c r="F81" s="30">
-        <v>2.56309423512967</v>
+        <v>0.834736056070392</v>
       </c>
       <c r="G81" s="43">
-        <v>2.83875265400528</v>
+        <v>0.88133802378095</v>
       </c>
       <c r="H81" s="43"/>
       <c r="I81" s="30">
-        <v>2.43914497442258</v>
+        <v>0.877460600655496</v>
       </c>
       <c r="J81" s="30">
-        <v>2.44006613749609</v>
+        <v>0.874248852668361</v>
       </c>
       <c r="K81" s="30">
-        <v>2.19457197019143</v>
+        <v>0.80613556286161</v>
       </c>
     </row>
     <row r="83" ht="28.5" customHeight="1">
@@ -4282,26 +4282,26 @@
       </c>
       <c r="C84" s="53"/>
       <c r="D84" s="11">
-        <v>106497</v>
+        <v>106497.017</v>
       </c>
       <c r="E84" s="12">
-        <v>5.65170446905198</v>
+        <v>5.6516608695246395</v>
       </c>
       <c r="F84" s="12">
-        <v>0.85989784845600625</v>
+        <v>0.85995368876758871</v>
       </c>
       <c r="G84" s="40">
-        <v>1.25820304257792</v>
+        <v>1.25820806415471</v>
       </c>
       <c r="H84" s="40"/>
       <c r="I84" s="12">
-        <v>26.304014267922572</v>
+        <v>26.304469288683819</v>
       </c>
       <c r="J84" s="12">
-        <v>-3.5399949869941</v>
+        <v>-3.54092652233559</v>
       </c>
       <c r="K84" s="12">
-        <v>1.38292194462477</v>
+        <v>1.38309737400802</v>
       </c>
     </row>
     <row r="85">
@@ -4310,26 +4310,26 @@
       </c>
       <c r="C85" s="53"/>
       <c r="D85" s="11">
-        <v>10009</v>
+        <v>10009.002</v>
       </c>
       <c r="E85" s="12">
-        <v>7.32340893195786</v>
+        <v>7.322738534771</v>
       </c>
       <c r="F85" s="12">
-        <v>2.044669986982186</v>
+        <v>2.0446539853956569</v>
       </c>
       <c r="G85" s="40">
-        <v>2.09106582076131</v>
+        <v>2.09106601129663</v>
       </c>
       <c r="H85" s="40"/>
       <c r="I85" s="12">
-        <v>53.0927746092832</v>
+        <v>53.092741882992179</v>
       </c>
       <c r="J85" s="12">
-        <v>-1.44911959027759</v>
+        <v>-1.44912323305461</v>
       </c>
       <c r="K85" s="12">
-        <v>8.15042539401015</v>
+        <v>8.15040691304201</v>
       </c>
     </row>
     <row r="86">
@@ -4338,26 +4338,26 @@
       </c>
       <c r="C86" s="53"/>
       <c r="D86" s="11">
-        <v>89439</v>
+        <v>89439.018</v>
       </c>
       <c r="E86" s="12">
-        <v>5.4551146591313406</v>
+        <v>5.45513984567675</v>
       </c>
       <c r="F86" s="12">
-        <v>0.700074860338396</v>
+        <v>0.70014349662084729</v>
       </c>
       <c r="G86" s="40">
-        <v>1.13336130964881</v>
+        <v>1.13336730591095</v>
       </c>
       <c r="H86" s="40"/>
       <c r="I86" s="12">
-        <v>21.500735082165058</v>
+        <v>21.501367680768357</v>
       </c>
       <c r="J86" s="12">
-        <v>-3.7330065997664</v>
+        <v>-3.73410889606725</v>
       </c>
       <c r="K86" s="12">
-        <v>0.62691224916184</v>
+        <v>0.627160289458723</v>
       </c>
     </row>
     <row r="87">

</xml_diff>

<commit_message>
update 202212 report files
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/202212/jsliu__bank_test_&_city_(HF)(202212)_DASHBOARD.xlsx
+++ b/lib/report/benchmark_report/web14/exl/202212/jsliu__bank_test_&_city_(HF)(202212)_DASHBOARD.xlsx
@@ -43,7 +43,7 @@
     <t>As of date: Dec, 2022</t>
   </si>
   <si>
-    <t>Printed on: 2023-02-10 14:32</t>
+    <t>Printed on: 2023-02-14 16:47</t>
   </si>
   <si>
     <t>Previous Cycle: Sep, 2022</t>
@@ -322,7 +322,7 @@
   </si>
   <si>
     <t xml:space="preserve">Earnings-at-Risk (EaR)
- NII: 5,604
+ NII: 5,602
  12 months horizon</t>
   </si>
   <si>
@@ -389,7 +389,7 @@
   </si>
   <si>
     <t xml:space="preserve">Earnings-at-Risk (EaR)
- NII: 10,684
+ NII: 10,681
  24 months horizon</t>
   </si>
   <si>
@@ -415,7 +415,7 @@
   </si>
   <si>
     <t xml:space="preserve">EVE at Risk
- EVE: 24,690
+ EVE: 24,687
  Duration: 4.67</t>
   </si>
   <si>
@@ -2592,13 +2592,13 @@
         <v>26</v>
       </c>
       <c r="B20" s="63">
-        <v>140621.017</v>
+        <v>140621</v>
       </c>
       <c r="C20" s="65">
-        <v>4.9354966622094594</v>
+        <v>4.93546648035313</v>
       </c>
       <c r="D20" s="66">
-        <v>2.30556272893264</v>
+        <v>2.30615760719703</v>
       </c>
       <c r="E20" s="62">
         <v>141538</v>
@@ -2614,13 +2614,13 @@
       </c>
       <c r="J20" s="45"/>
       <c r="K20" s="58">
-        <v>17.543308486614002</v>
+        <v>17.5412243670937</v>
       </c>
       <c r="L20" s="15">
         <v>17.704968378931298</v>
       </c>
       <c r="M20" s="15">
-        <v>-0.16165989231729583</v>
+        <v>-0.16374401183759701</v>
       </c>
     </row>
     <row r="21">
@@ -2650,13 +2650,13 @@
       </c>
       <c r="J21" s="45"/>
       <c r="K21" s="58">
-        <v>4.66836062820837</v>
+        <v>4.67110368576127</v>
       </c>
       <c r="L21" s="15">
         <v>4.85617165336736</v>
       </c>
       <c r="M21" s="15">
-        <v>-0.1878110251589904</v>
+        <v>-0.18506796760608957</v>
       </c>
     </row>
     <row r="22">
@@ -2667,10 +2667,10 @@
         <v>16619</v>
       </c>
       <c r="C22" s="72">
-        <v>1.92724810999458</v>
+        <v>1.9267140678204502</v>
       </c>
       <c r="D22" s="70">
-        <v>1.46269349635631</v>
+        <v>1.46271404410312</v>
       </c>
       <c r="E22" s="67">
         <v>23708</v>
@@ -2686,13 +2686,13 @@
       </c>
       <c r="J22" s="45"/>
       <c r="K22" s="59">
-        <v>-22.8751582644323</v>
+        <v>-22.8685861410605</v>
       </c>
       <c r="L22" s="15">
         <v>-23.6586049659914</v>
       </c>
       <c r="M22" s="15">
-        <v>0.78344670155910023</v>
+        <v>0.79001882493090037</v>
       </c>
     </row>
     <row r="23">
@@ -2700,13 +2700,13 @@
         <v>32</v>
       </c>
       <c r="B23" s="68">
-        <v>106497.017</v>
+        <v>106497</v>
       </c>
       <c r="C23" s="70">
-        <v>5.6516608695246395</v>
-      </c>
-      <c r="D23" s="70">
-        <v>2.81624329385909</v>
+        <v>5.65170446905198</v>
+      </c>
+      <c r="D23" s="72">
+        <v>2.81703786070771</v>
       </c>
       <c r="E23" s="67">
         <v>104979</v>
@@ -2722,13 +2722,13 @@
       </c>
       <c r="J23" s="45"/>
       <c r="K23" s="58">
-        <v>7.20918749362305</v>
+        <v>7.2130362071470193</v>
       </c>
       <c r="L23" s="15">
         <v>8.48120704617382</v>
       </c>
       <c r="M23" s="15">
-        <v>-1.2720195525507698</v>
+        <v>-1.2681708390268005</v>
       </c>
     </row>
     <row r="24">
@@ -2736,13 +2736,13 @@
         <v>34</v>
       </c>
       <c r="B24" s="68">
-        <v>89439.018</v>
+        <v>89439</v>
       </c>
       <c r="C24" s="72">
-        <v>5.45513984567675</v>
+        <v>5.4551146591313406</v>
       </c>
       <c r="D24" s="70">
-        <v>2.9414018645567</v>
+        <v>2.94234700490486</v>
       </c>
       <c r="E24" s="67">
         <v>88990</v>
@@ -2758,13 +2758,13 @@
       </c>
       <c r="J24" s="45"/>
       <c r="K24" s="60">
-        <v>915.825026118946</v>
+        <v>915.765411670193</v>
       </c>
       <c r="L24" s="28">
         <v>900.441476372895</v>
       </c>
       <c r="M24" s="28">
-        <v>15.383549746051017</v>
+        <v>15.323935297298021</v>
       </c>
     </row>
     <row r="25">
@@ -2772,13 +2772,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="68">
-        <v>17057.999</v>
+        <v>17058</v>
       </c>
       <c r="C25" s="70">
-        <v>6.6777270565712907</v>
+        <v>6.67812880335631</v>
       </c>
       <c r="D25" s="72">
-        <v>2.17473224911237</v>
+        <v>2.17478046521023</v>
       </c>
       <c r="E25" s="67">
         <v>15989</v>
@@ -2794,13 +2794,13 @@
       </c>
       <c r="J25" s="45"/>
       <c r="K25" s="58">
-        <v>4.09612969763073</v>
+        <v>4.0949647963934</v>
       </c>
       <c r="L25" s="15">
         <v>4.20927007445733</v>
       </c>
       <c r="M25" s="15">
-        <v>-0.11314037682659972</v>
+        <v>-0.11430527806392998</v>
       </c>
     </row>
     <row r="26" ht="15">
@@ -2808,13 +2808,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="63">
-        <v>124823.003</v>
+        <v>124823</v>
       </c>
       <c r="C26" s="65">
-        <v>0.537152610084218</v>
+        <v>0.538257319138784</v>
       </c>
       <c r="D26" s="66">
-        <v>1.80285892554534</v>
+        <v>1.80306925229776</v>
       </c>
       <c r="E26" s="62">
         <v>126134</v>
@@ -2830,13 +2830,13 @@
       </c>
       <c r="J26" s="45"/>
       <c r="K26" s="61">
-        <v>5603.78112555724</v>
+        <v>5602.16442647506</v>
       </c>
       <c r="L26" s="28">
         <v>5815.23232341052</v>
       </c>
       <c r="M26" s="28">
-        <v>-211.45119785328006</v>
+        <v>-213.06789693545943</v>
       </c>
     </row>
     <row r="27">
@@ -2844,13 +2844,13 @@
         <v>40</v>
       </c>
       <c r="B27" s="71">
-        <v>120242.999</v>
+        <v>120243</v>
       </c>
       <c r="C27" s="72">
-        <v>0.545636784225584</v>
+        <v>0.546637665111986</v>
       </c>
       <c r="D27" s="70">
-        <v>1.85057233385735</v>
+        <v>1.85079208093601</v>
       </c>
       <c r="E27" s="67">
         <v>125524</v>
@@ -2866,13 +2866,13 @@
       </c>
       <c r="J27" s="45"/>
       <c r="K27" s="61">
-        <v>1137.05809946493</v>
+        <v>1135.84533810065</v>
       </c>
       <c r="L27" s="28">
         <v>1518.9642274414</v>
       </c>
       <c r="M27" s="28">
-        <v>-381.90612797647009</v>
+        <v>-383.11888934075</v>
       </c>
     </row>
     <row r="28">
@@ -2883,10 +2883,10 @@
         <v>83018</v>
       </c>
       <c r="C28" s="72">
-        <v>0.36069566984219803</v>
+        <v>0.362187791786938</v>
       </c>
       <c r="D28" s="72">
-        <v>2.38175694478556</v>
+        <v>2.38207397259864</v>
       </c>
       <c r="E28" s="67">
         <v>88201</v>
@@ -2902,13 +2902,13 @@
       </c>
       <c r="J28" s="45"/>
       <c r="K28" s="58">
-        <v>4.60532493145209</v>
+        <v>4.60104108551501</v>
       </c>
       <c r="L28" s="15">
         <v>6.02576525365789</v>
       </c>
       <c r="M28" s="15">
-        <v>-1.4204403222058</v>
+        <v>-1.4247241681428804</v>
       </c>
     </row>
     <row r="29">
@@ -2916,13 +2916,13 @@
         <v>44</v>
       </c>
       <c r="B29" s="71">
-        <v>37224.999</v>
+        <v>37225</v>
       </c>
       <c r="C29" s="72">
-        <v>0.951879764993416</v>
+        <v>0.951762330869526</v>
       </c>
       <c r="D29" s="70">
-        <v>0.737415558666343</v>
+        <v>0.737428575316329</v>
       </c>
       <c r="E29" s="67">
         <v>37323</v>
@@ -2939,13 +2939,13 @@
         <v>45</v>
       </c>
       <c r="B30" s="68">
-        <v>4199.004</v>
+        <v>4199</v>
       </c>
       <c r="C30" s="72">
-        <v>0.342938125326863</v>
+        <v>0.347116118313884</v>
       </c>
       <c r="D30" s="72">
-        <v>0.663581364719357</v>
+        <v>0.66356921704137</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>46</v>
@@ -3028,7 +3028,7 @@
         <v>400</v>
       </c>
       <c r="D35" s="19">
-        <v>0.0720918749362305</v>
+        <v>0.0721303620714702</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>57</v>
@@ -3052,7 +3052,7 @@
         <v>300</v>
       </c>
       <c r="D36" s="19">
-        <v>0.0560271290432385</v>
+        <v>0.0560613395931156</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>57</v>
@@ -3076,7 +3076,7 @@
         <v>200</v>
       </c>
       <c r="D37" s="19">
-        <v>0.0396517140342517</v>
+        <v>0.039678797388226</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>57</v>
@@ -3108,7 +3108,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="19">
-        <v>0.0208057514968031</v>
+        <v>0.020817395128413</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>57</v>
@@ -3166,7 +3166,7 @@
         <v>-100</v>
       </c>
       <c r="D40" s="19">
-        <v>-0.0221050584631583</v>
+        <v>-0.0221122048653095</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>57</v>
@@ -3198,7 +3198,7 @@
         <v>-200</v>
       </c>
       <c r="D41" s="19">
-        <v>-0.0459758490133388</v>
+        <v>-0.0459949505910554</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>57</v>
@@ -3252,7 +3252,7 @@
         <v>67</v>
       </c>
       <c r="D43" s="19">
-        <v>0.0346064322747612</v>
+        <v>0.034631821104308</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>57</v>
@@ -3314,7 +3314,7 @@
         <v>400</v>
       </c>
       <c r="D45" s="19">
-        <v>0.112392266037563</v>
+        <v>0.112453631813822</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>57</v>
@@ -3346,7 +3346,7 @@
         <v>300</v>
       </c>
       <c r="D46" s="19">
-        <v>0.0882774689802363</v>
+        <v>0.0883316509268715</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>57</v>
@@ -3378,7 +3378,7 @@
         <v>200</v>
       </c>
       <c r="D47" s="19">
-        <v>0.0628096688695394</v>
+        <v>0.0628510983601754</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>57</v>
@@ -3410,7 +3410,7 @@
         <v>100</v>
       </c>
       <c r="D48" s="19">
-        <v>0.0327354849332773</v>
+        <v>0.0327497493573731</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>57</v>
@@ -3466,7 +3466,7 @@
         <v>-100</v>
       </c>
       <c r="D50" s="19">
-        <v>-0.0351775880960924</v>
+        <v>-0.0351894510558918</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>57</v>
@@ -3498,7 +3498,7 @@
         <v>-200</v>
       </c>
       <c r="D51" s="19">
-        <v>-0.074364645368532</v>
+        <v>-0.0743953789622909</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>57</v>
@@ -3544,7 +3544,7 @@
         <v>67</v>
       </c>
       <c r="D53" s="19">
-        <v>0.0413423340460545</v>
+        <v>0.0413740549447014</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>57</v>
@@ -3595,7 +3595,7 @@
         <v>400</v>
       </c>
       <c r="D55" s="19">
-        <v>-0.228751582644323</v>
+        <v>-0.228685861410605</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>57</v>
@@ -3619,7 +3619,7 @@
         <v>300</v>
       </c>
       <c r="D56" s="19">
-        <v>-0.166440467163279</v>
+        <v>-0.166379821983069</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>57</v>
@@ -3643,7 +3643,7 @@
         <v>200</v>
       </c>
       <c r="D57" s="19">
-        <v>-0.104776741352632</v>
+        <v>-0.104730579047761</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>57</v>
@@ -3675,7 +3675,7 @@
         <v>100</v>
       </c>
       <c r="D58" s="19">
-        <v>-0.0500038327141156</v>
+        <v>-0.0499840855492294</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>57</v>
@@ -3691,13 +3691,13 @@
       </c>
       <c r="J58" s="45"/>
       <c r="K58" s="15">
-        <v>7.8042447741574</v>
+        <v>7.8041421168346909</v>
       </c>
       <c r="L58" s="15">
-        <v>7.82891202706346</v>
+        <v>7.8288089648115591</v>
       </c>
       <c r="M58" s="15">
-        <v>25.2128308079875</v>
+        <v>25.2028458491224</v>
       </c>
     </row>
     <row r="59" ht="15">
@@ -3717,13 +3717,13 @@
       </c>
       <c r="J59" s="45"/>
       <c r="K59" s="15">
-        <v>18.092554084594</v>
+        <v>18.092224534714298</v>
       </c>
       <c r="L59" s="15">
-        <v>18.166891985577</v>
+        <v>18.16656048182</v>
       </c>
       <c r="M59" s="15">
-        <v>40.8238246105632</v>
+        <v>40.813697746016096</v>
       </c>
     </row>
     <row r="60" ht="15">
@@ -3733,7 +3733,7 @@
         <v>-100</v>
       </c>
       <c r="D60" s="19">
-        <v>0.0431157477391154</v>
+        <v>0.0430980873185049</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>57</v>
@@ -3749,13 +3749,13 @@
       </c>
       <c r="J60" s="45"/>
       <c r="K60" s="15">
-        <v>2.31116498749648</v>
+        <v>2.31111719823051</v>
       </c>
       <c r="L60" s="15">
-        <v>2.31730188347427</v>
+        <v>2.31725395626537</v>
       </c>
       <c r="M60" s="15">
-        <v>26.5780875530575</v>
+        <v>26.5638157029415</v>
       </c>
     </row>
     <row r="61" ht="15">
@@ -3765,7 +3765,7 @@
         <v>-200</v>
       </c>
       <c r="D61" s="19">
-        <v>0.0691119416445477</v>
+        <v>0.069107962235365</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>57</v>
@@ -3793,7 +3793,7 @@
         <v>67</v>
       </c>
       <c r="D63" s="19">
-        <v>-0.0831690682530268</v>
+        <v>-0.0831664613020303</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>57</v>
@@ -3842,20 +3842,20 @@
         <v>13100</v>
       </c>
       <c r="F66" s="16">
-        <v>13236.9400546305</v>
+        <v>13236.851525381</v>
       </c>
       <c r="G66" s="42">
-        <v>13349.2870445035</v>
+        <v>13349.1075948985</v>
       </c>
       <c r="H66" s="42"/>
       <c r="I66" s="16">
-        <v>13461.7427823901</v>
+        <v>13461.4644358334</v>
       </c>
       <c r="J66" s="16">
-        <v>13570.7480648864</v>
+        <v>13570.3639992764</v>
       </c>
       <c r="K66" s="16">
-        <v>13673.3041714</v>
+        <v>13672.81511447</v>
       </c>
     </row>
     <row r="67">
@@ -3865,23 +3865,23 @@
       <c r="C67" s="44"/>
       <c r="D67" s="44"/>
       <c r="E67" s="16">
-        <v>207.349645340184</v>
+        <v>207.349356204663</v>
       </c>
       <c r="F67" s="16">
-        <v>1613.40565657602</v>
+        <v>1613.40566644065</v>
       </c>
       <c r="G67" s="42">
-        <v>208.060433806942</v>
+        <v>208.060144157945</v>
       </c>
       <c r="H67" s="42"/>
       <c r="I67" s="16">
-        <v>247.128459750317</v>
+        <v>247.12825661806</v>
       </c>
       <c r="J67" s="16">
-        <v>272.551887845893</v>
+        <v>272.55215200818</v>
       </c>
       <c r="K67" s="16">
-        <v>2434.7284369987</v>
+        <v>2434.72792815442</v>
       </c>
     </row>
     <row r="68">
@@ -3891,23 +3891,23 @@
       <c r="C68" s="44"/>
       <c r="D68" s="44"/>
       <c r="E68" s="16">
-        <v>1936.58608054635</v>
+        <v>1937.19853524096</v>
       </c>
       <c r="F68" s="16">
-        <v>1658.91798905265</v>
+        <v>1660.05501576672</v>
       </c>
       <c r="G68" s="42">
-        <v>1864.19802511673</v>
+        <v>1865.75178856004</v>
       </c>
       <c r="H68" s="42"/>
       <c r="I68" s="16">
-        <v>1931.31043378126</v>
+        <v>1931.9491893882</v>
       </c>
       <c r="J68" s="16">
-        <v>1999.15349596587</v>
+        <v>1999.39644746939</v>
       </c>
       <c r="K68" s="16">
-        <v>1893.18904989299</v>
+        <v>1893.33288243763</v>
       </c>
     </row>
     <row r="69">
@@ -3916,24 +3916,24 @@
       </c>
       <c r="C69" s="44"/>
       <c r="D69" s="44"/>
-      <c r="E69" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G69" s="42" t="s">
-        <v>46</v>
+      <c r="E69" s="16">
+        <v>333.333333333333</v>
+      </c>
+      <c r="F69" s="16">
+        <v>666.666666666663</v>
+      </c>
+      <c r="G69" s="42">
+        <v>666.666666666663</v>
       </c>
       <c r="H69" s="42"/>
-      <c r="I69" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J69" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="K69" s="16" t="s">
-        <v>46</v>
+      <c r="I69" s="16">
+        <v>666.666666666673</v>
+      </c>
+      <c r="J69" s="16">
+        <v>666.666666666663</v>
+      </c>
+      <c r="K69" s="16">
+        <v>666.666666666663</v>
       </c>
     </row>
     <row r="70">
@@ -3943,23 +3943,23 @@
       <c r="C70" s="44"/>
       <c r="D70" s="44"/>
       <c r="E70" s="16">
-        <v>4623.81378528582</v>
+        <v>4622.98866130839</v>
       </c>
       <c r="F70" s="16">
-        <v>4600.87718088603</v>
+        <v>4600.05359122427</v>
       </c>
       <c r="G70" s="42">
-        <v>4581.3145533773</v>
+        <v>4580.4976115504</v>
       </c>
       <c r="H70" s="42"/>
       <c r="I70" s="16">
-        <v>6584.51757328417</v>
+        <v>6583.71868809411</v>
       </c>
       <c r="J70" s="16">
-        <v>6556.77137905015</v>
+        <v>6555.95915484407</v>
       </c>
       <c r="K70" s="16">
-        <v>6531.64105017944</v>
+        <v>6530.81449052776</v>
       </c>
     </row>
     <row r="71">
@@ -3969,23 +3969,23 @@
       <c r="C71" s="44"/>
       <c r="D71" s="44"/>
       <c r="E71" s="16">
-        <v>136.940054630411</v>
+        <v>136.851525380826</v>
       </c>
       <c r="F71" s="16">
-        <v>112.346990171524</v>
+        <v>112.256069815983</v>
       </c>
       <c r="G71" s="42">
-        <v>112.455736835422</v>
+        <v>112.356839883678</v>
       </c>
       <c r="H71" s="42"/>
       <c r="I71" s="16">
-        <v>109.005281139708</v>
+        <v>108.899562086538</v>
       </c>
       <c r="J71" s="16">
-        <v>102.556107116348</v>
+        <v>102.451115796415</v>
       </c>
       <c r="K71" s="16">
-        <v>95.3787549543705</v>
+        <v>95.2742607676718</v>
       </c>
     </row>
     <row r="72">
@@ -4021,23 +4021,23 @@
       <c r="C73" s="45"/>
       <c r="D73" s="45"/>
       <c r="E73" s="16">
-        <v>15380.8757805169</v>
+        <v>20337.7214114682</v>
       </c>
       <c r="F73" s="16">
-        <v>16621.6106904307</v>
+        <v>21889.2885352952</v>
       </c>
       <c r="G73" s="42">
-        <v>15534.0012402625</v>
+        <v>20782.4406457172</v>
       </c>
       <c r="H73" s="42"/>
       <c r="I73" s="16">
-        <v>15749.1869570614</v>
+        <v>22999.8267986869</v>
       </c>
       <c r="J73" s="16">
-        <v>15945.0095558145</v>
+        <v>23167.3895360611</v>
       </c>
       <c r="K73" s="16">
-        <v>18096.600413246</v>
+        <v>25293.6313430241</v>
       </c>
     </row>
     <row r="74">
@@ -4047,23 +4047,23 @@
       <c r="C74" s="44"/>
       <c r="D74" s="44"/>
       <c r="E74" s="16">
-        <v>207.349645340184</v>
+        <v>207.349356204654</v>
       </c>
       <c r="F74" s="16">
-        <v>1613.40565657591</v>
+        <v>1613.40566644054</v>
       </c>
       <c r="G74" s="42">
-        <v>208.060433806788</v>
+        <v>208.060144157792</v>
       </c>
       <c r="H74" s="42"/>
       <c r="I74" s="16">
-        <v>247.128459751007</v>
+        <v>247.128256618752</v>
       </c>
       <c r="J74" s="16">
-        <v>272.551887845698</v>
+        <v>272.552152007986</v>
       </c>
       <c r="K74" s="16">
-        <v>2434.72843699826</v>
+        <v>2434.72792815398</v>
       </c>
     </row>
     <row r="75">
@@ -4073,23 +4073,23 @@
       <c r="C75" s="44"/>
       <c r="D75" s="44"/>
       <c r="E75" s="16">
-        <v>1954.40019552537</v>
+        <v>1955.01263724983</v>
       </c>
       <c r="F75" s="16">
-        <v>1677.39856526427</v>
+        <v>1678.53557759155</v>
       </c>
       <c r="G75" s="42">
-        <v>1883.4132516961</v>
+        <v>1884.96699133093</v>
       </c>
       <c r="H75" s="42"/>
       <c r="I75" s="16">
-        <v>1952.28186965485</v>
+        <v>1952.92066048745</v>
       </c>
       <c r="J75" s="16">
-        <v>2020.96355722983</v>
+        <v>2021.2065837925</v>
       </c>
       <c r="K75" s="16">
-        <v>1917.25330725089</v>
+        <v>1917.39732064392</v>
       </c>
     </row>
     <row r="76">
@@ -4099,23 +4099,23 @@
       <c r="C76" s="44"/>
       <c r="D76" s="44"/>
       <c r="E76" s="16">
-        <v>333.333</v>
+        <v>333.333333333333</v>
       </c>
       <c r="F76" s="16">
-        <v>666.666</v>
+        <v>666.666666666666</v>
       </c>
       <c r="G76" s="42">
-        <v>666.666</v>
+        <v>666.666666666666</v>
       </c>
       <c r="H76" s="42"/>
       <c r="I76" s="16">
-        <v>666.666</v>
+        <v>666.666666666666</v>
       </c>
       <c r="J76" s="16">
-        <v>666.666</v>
+        <v>666.666666666666</v>
       </c>
       <c r="K76" s="16">
-        <v>666.666</v>
+        <v>666.666666666666</v>
       </c>
     </row>
     <row r="77">
@@ -4125,23 +4125,23 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="16">
-        <v>4623.81378528572</v>
+        <v>4622.98866130831</v>
       </c>
       <c r="F77" s="16">
-        <v>4600.87718121602</v>
+        <v>4600.05359155425</v>
       </c>
       <c r="G77" s="42">
-        <v>4581.31455225658</v>
+        <v>4580.49761042952</v>
       </c>
       <c r="H77" s="42"/>
       <c r="I77" s="16">
-        <v>6584.51757196881</v>
+        <v>6583.71868677884</v>
       </c>
       <c r="J77" s="16">
-        <v>6556.77137970991</v>
+        <v>6555.95915550386</v>
       </c>
       <c r="K77" s="16">
-        <v>6531.64104984629</v>
+        <v>6530.81449019453</v>
       </c>
     </row>
     <row r="78">
@@ -4151,23 +4151,23 @@
       <c r="C78" s="44"/>
       <c r="D78" s="44"/>
       <c r="E78" s="16">
-        <v>-17.8141149790485</v>
+        <v>-17.8141020089245</v>
       </c>
       <c r="F78" s="16">
-        <v>-18.480576242902</v>
+        <v>-18.4805618562523</v>
       </c>
       <c r="G78" s="42">
-        <v>-19.215226509743</v>
+        <v>-19.2152027010538</v>
       </c>
       <c r="H78" s="42"/>
       <c r="I78" s="16">
-        <v>-20.9714359154992</v>
+        <v>-20.9714711411306</v>
       </c>
       <c r="J78" s="16">
-        <v>-21.8100613207209</v>
+        <v>-21.8101363799145</v>
       </c>
       <c r="K78" s="16">
-        <v>-24.064257363565</v>
+        <v>-24.0644382121033</v>
       </c>
     </row>
     <row r="79">
@@ -4203,23 +4203,23 @@
       <c r="C80" s="46"/>
       <c r="D80" s="46"/>
       <c r="E80" s="16">
-        <v>17542.6256213826</v>
+        <v>7100.86988608712</v>
       </c>
       <c r="F80" s="16">
-        <v>19912.4149119408</v>
+        <v>8540.18094039677</v>
       </c>
       <c r="G80" s="42">
-        <v>17625.4749268862</v>
+        <v>7320.97620988384</v>
       </c>
       <c r="H80" s="42"/>
       <c r="I80" s="16">
-        <v>17948.5972877827</v>
+        <v>9429.46279941057</v>
       </c>
       <c r="J80" s="16">
-        <v>18238.5250002303</v>
+        <v>9494.57442159112</v>
       </c>
       <c r="K80" s="16">
-        <v>22448.5821578282</v>
+        <v>11525.541967447</v>
       </c>
     </row>
     <row r="81">
@@ -4229,23 +4229,23 @@
       <c r="C81" s="46"/>
       <c r="D81" s="46"/>
       <c r="E81" s="30">
-        <v>0.87677159123599</v>
+        <v>2.86411689521537</v>
       </c>
       <c r="F81" s="30">
-        <v>0.834736056070392</v>
+        <v>2.56309423512967</v>
       </c>
       <c r="G81" s="43">
-        <v>0.88133802378095</v>
+        <v>2.83875265400528</v>
       </c>
       <c r="H81" s="43"/>
       <c r="I81" s="30">
-        <v>0.877460600655496</v>
+        <v>2.43914497442258</v>
       </c>
       <c r="J81" s="30">
-        <v>0.874248852668361</v>
+        <v>2.44006613749609</v>
       </c>
       <c r="K81" s="30">
-        <v>0.80613556286161</v>
+        <v>2.19457197019143</v>
       </c>
     </row>
     <row r="83" ht="28.5" customHeight="1">
@@ -4282,26 +4282,26 @@
       </c>
       <c r="C84" s="53"/>
       <c r="D84" s="11">
-        <v>106497.017</v>
+        <v>106497</v>
       </c>
       <c r="E84" s="12">
-        <v>5.6516608695246395</v>
+        <v>5.65170446905198</v>
       </c>
       <c r="F84" s="12">
-        <v>0.85995368876758871</v>
+        <v>0.85989784845600625</v>
       </c>
       <c r="G84" s="40">
-        <v>1.25820806415471</v>
+        <v>1.25820304257792</v>
       </c>
       <c r="H84" s="40"/>
       <c r="I84" s="12">
-        <v>26.304469288683819</v>
+        <v>26.304014267922572</v>
       </c>
       <c r="J84" s="12">
-        <v>-3.54092652233559</v>
+        <v>-3.5399949869941</v>
       </c>
       <c r="K84" s="12">
-        <v>1.38309737400802</v>
+        <v>1.38292194462477</v>
       </c>
     </row>
     <row r="85">
@@ -4310,26 +4310,26 @@
       </c>
       <c r="C85" s="53"/>
       <c r="D85" s="11">
-        <v>10009.002</v>
+        <v>10009</v>
       </c>
       <c r="E85" s="12">
-        <v>7.322738534771</v>
+        <v>7.32340893195786</v>
       </c>
       <c r="F85" s="12">
-        <v>2.0446539853956569</v>
+        <v>2.044669986982186</v>
       </c>
       <c r="G85" s="40">
-        <v>2.09106601129663</v>
+        <v>2.09106582076131</v>
       </c>
       <c r="H85" s="40"/>
       <c r="I85" s="12">
-        <v>53.092741882992179</v>
+        <v>53.0927746092832</v>
       </c>
       <c r="J85" s="12">
-        <v>-1.44912323305461</v>
+        <v>-1.44911959027759</v>
       </c>
       <c r="K85" s="12">
-        <v>8.15040691304201</v>
+        <v>8.15042539401015</v>
       </c>
     </row>
     <row r="86">
@@ -4338,26 +4338,26 @@
       </c>
       <c r="C86" s="53"/>
       <c r="D86" s="11">
-        <v>89439.018</v>
+        <v>89439</v>
       </c>
       <c r="E86" s="12">
-        <v>5.45513984567675</v>
+        <v>5.4551146591313406</v>
       </c>
       <c r="F86" s="12">
-        <v>0.70014349662084729</v>
+        <v>0.700074860338396</v>
       </c>
       <c r="G86" s="40">
-        <v>1.13336730591095</v>
+        <v>1.13336130964881</v>
       </c>
       <c r="H86" s="40"/>
       <c r="I86" s="12">
-        <v>21.501367680768357</v>
+        <v>21.500735082165058</v>
       </c>
       <c r="J86" s="12">
-        <v>-3.73410889606725</v>
+        <v>-3.7330065997664</v>
       </c>
       <c r="K86" s="12">
-        <v>0.627160289458723</v>
+        <v>0.62691224916184</v>
       </c>
     </row>
     <row r="87">

</xml_diff>